<commit_message>
Añadiendo nuevas funcionalidades y modificando el proyecto
</commit_message>
<xml_diff>
--- a/CapstoneProject/sorte/datos.xlsx
+++ b/CapstoneProject/sorte/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -465,16 +465,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>